<commit_message>
removed trial pages and tests. Added basic pages for sauce demo and a sample test; updated config file to point to saucedemo site; added a element present check method in base page; updated class name in testng test suite
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CodeRepo\TestRepo\SeleniumAutomationFramework\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DemoGitHub\SeleniumAutomationFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C169A963-0C64-451C-B644-B81921C6B2DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F131EA-EEEE-4474-84A1-8DBB7FA1F92B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D9AE0F58-2579-4A19-BFE7-108FD11782DA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D9AE0F58-2579-4A19-BFE7-108FD11782DA}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>testname</t>
   </si>
@@ -56,18 +56,9 @@
     <t>loginLogoutTest</t>
   </si>
   <si>
-    <t>newTest</t>
-  </si>
-  <si>
     <t>To check whether the user can successfully login and logout</t>
   </si>
   <si>
-    <t>To check whether this is executed</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -80,49 +71,19 @@
     <t>password</t>
   </si>
   <si>
-    <t>fname</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>admin123</t>
-  </si>
-  <si>
-    <t>sujay</t>
-  </si>
-  <si>
-    <t>sb</t>
-  </si>
-  <si>
-    <t>testsb</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
     <t>browser</t>
   </si>
   <si>
     <t>chrome</t>
   </si>
   <si>
-    <t>firefox</t>
-  </si>
-  <si>
-    <t>Test Amazon India</t>
-  </si>
-  <si>
-    <t>amazonTest</t>
-  </si>
-  <si>
-    <t>Laptops</t>
-  </si>
-  <si>
-    <t>menutext</t>
+    <t>standard_user</t>
+  </si>
+  <si>
+    <t>secret_sauce</t>
+  </si>
+  <si>
+    <t>locked_out_user</t>
   </si>
 </sst>
 </file>
@@ -158,11 +119,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7276309-7F10-481B-BE1E-97A4DCAD8700}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,50 +472,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -565,15 +491,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{094BECEF-4844-4418-B6F1-0C40CA92EC6D}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -581,157 +507,47 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
       <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added pages for cart, product and header and menu. Added a test to add to cart updated pom to use webdriver manager.
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DemoGitHub\SeleniumAutomationFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F131EA-EEEE-4474-84A1-8DBB7FA1F92B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C470C7D-E6AD-4BE5-88FD-BB7DB8104FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D9AE0F58-2579-4A19-BFE7-108FD11782DA}"/>
+    <workbookView xWindow="-6240" yWindow="-12495" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{D9AE0F58-2579-4A19-BFE7-108FD11782DA}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>testname</t>
   </si>
@@ -83,7 +83,10 @@
     <t>secret_sauce</t>
   </si>
   <si>
-    <t>locked_out_user</t>
+    <t>addItemsToCartTest</t>
+  </si>
+  <si>
+    <t>To check whether the user can add items to cart</t>
   </si>
 </sst>
 </file>
@@ -437,20 +440,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7276309-7F10-481B-BE1E-97A4DCAD8700}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:H1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="24.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="24.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" style="1"/>
-    <col min="2" max="2" width="55.28515625" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="24.42578125" style="1"/>
+    <col min="1" max="1" width="24.44140625" style="1"/>
+    <col min="2" max="2" width="55.33203125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="24.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -467,7 +470,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -481,6 +484,23 @@
         <v>7</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -493,13 +513,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{094BECEF-4844-4418-B6F1-0C40CA92EC6D}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="27.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="27.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -516,7 +536,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -533,9 +553,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>15</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -544,7 +564,7 @@
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>
@@ -552,5 +572,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added some functionality for cart page, updated test case
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DemoGitHub\SeleniumAutomationFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C470C7D-E6AD-4BE5-88FD-BB7DB8104FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{034F7084-ACB8-4BD7-9E2E-51F162902CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6240" yWindow="-12495" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{D9AE0F58-2579-4A19-BFE7-108FD11782DA}"/>
+    <workbookView xWindow="13830" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D9AE0F58-2579-4A19-BFE7-108FD11782DA}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
   <si>
     <t>testname</t>
   </si>
@@ -87,6 +87,30 @@
   </si>
   <si>
     <t>To check whether the user can add items to cart</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Sauce Labs Backpack</t>
+  </si>
+  <si>
+    <t>items</t>
+  </si>
+  <si>
+    <t>Sauce Labs Bike Light, Sauce Labs Backpack</t>
+  </si>
+  <si>
+    <t>Sauce Labs Backpack, Test.allTheThings() T-Shirt (Red)</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>problem_user</t>
+  </si>
+  <si>
+    <t>performance_glitch_user</t>
   </si>
 </sst>
 </file>
@@ -122,10 +146,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,7 +468,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -478,7 +503,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>7</v>
@@ -511,15 +536,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{094BECEF-4844-4418-B6F1-0C40CA92EC6D}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="48.21875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -535,13 +563,16 @@
       <c r="E1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -552,8 +583,11 @@
       <c r="E2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -568,6 +602,49 @@
       </c>
       <c r="E3" t="s">
         <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed failing tests; removed chaining for navigation; added feature to slow down test execution.
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DemoGitHub\SeleniumAutomationFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8679E4CC-0287-4C0A-9661-D758E6FAE0BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD7FFFF-002A-4520-86A9-B113AFD97F6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13830" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D9AE0F58-2579-4A19-BFE7-108FD11782DA}"/>
+    <workbookView xWindow="-14970" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D9AE0F58-2579-4A19-BFE7-108FD11782DA}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="36">
   <si>
     <t>testname</t>
   </si>
@@ -110,10 +110,40 @@
     <t>Verify that user is able to add items and proceed to checkout with valid user login</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Sauce Labs Fleece Jacket; Test.allTheThings() T-Shirt (Red)</t>
+    <t>invalidDeliveryAddress</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Test invalid delivery details</t>
+  </si>
+  <si>
+    <t>Sauce Labs Fleece Jacket</t>
+  </si>
+  <si>
+    <t>firefox</t>
+  </si>
+  <si>
+    <t>0628</t>
+  </si>
+  <si>
+    <t>1010</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Wick</t>
+  </si>
+  <si>
+    <t>Ethan</t>
+  </si>
+  <si>
+    <t>Hunt</t>
+  </si>
+  <si>
+    <t>Sauce Labs Fleece Jacket;Test.allTheThings() T-Shirt (Red)</t>
   </si>
 </sst>
 </file>
@@ -468,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7276309-7F10-481B-BE1E-97A4DCAD8700}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -523,12 +553,29 @@
         <v>23</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -540,10 +587,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{094BECEF-4844-4418-B6F1-0C40CA92EC6D}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -617,7 +664,7 @@
         <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
         <v>21</v>
@@ -646,7 +693,7 @@
         <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
@@ -655,15 +702,73 @@
         <v>11</v>
       </c>
       <c r="F4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" s="3" t="s">
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated test data sheet. corrected the JsExecutor arguments.
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DemoGitHub\SeleniumAutomationFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD7FFFF-002A-4520-86A9-B113AFD97F6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B6270C-7F89-4C32-B88D-1886297CC7E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14970" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D9AE0F58-2579-4A19-BFE7-108FD11782DA}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D9AE0F58-2579-4A19-BFE7-108FD11782DA}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="46">
   <si>
     <t>testname</t>
   </si>
@@ -92,9 +92,6 @@
     <t>invalidCredentialsTest</t>
   </si>
   <si>
-    <t>Verify that user is unable to Buy items on SauceDemo with invalid credentials</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
@@ -107,18 +104,9 @@
     <t>addItemsToCartTest</t>
   </si>
   <si>
-    <t>Verify that user is able to add items and proceed to checkout with valid user login</t>
-  </si>
-  <si>
     <t>invalidDeliveryAddress</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>Test invalid delivery details</t>
-  </si>
-  <si>
     <t>Sauce Labs Fleece Jacket</t>
   </si>
   <si>
@@ -144,6 +132,48 @@
   </si>
   <si>
     <t>Sauce Labs Fleece Jacket;Test.allTheThings() T-Shirt (Red)</t>
+  </si>
+  <si>
+    <t>checkoutWithEmptyCart</t>
+  </si>
+  <si>
+    <t>QE-26 Verify that user is able to add items and proceed to checkout with valid user login</t>
+  </si>
+  <si>
+    <t>QE-27 Verify that user is unable to Buy items on SauceDemo with invalid credentials</t>
+  </si>
+  <si>
+    <t>QE-29 Verify that user is unable to checkout with empty cart</t>
+  </si>
+  <si>
+    <t>performance_glitch_user</t>
+  </si>
+  <si>
+    <t>problem_user</t>
+  </si>
+  <si>
+    <t>Aaron</t>
+  </si>
+  <si>
+    <t>Finch</t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>123!!</t>
+  </si>
+  <si>
+    <t>32432!!</t>
+  </si>
+  <si>
+    <t>!!!!!</t>
+  </si>
+  <si>
+    <t>QE-28 Verify that user is unable to checkout with invalid delivery details</t>
   </si>
 </sst>
 </file>
@@ -498,20 +528,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7276309-7F10-481B-BE1E-97A4DCAD8700}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="24.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="24.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.44140625" style="1"/>
-    <col min="2" max="2" width="68.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="24.44140625" style="1"/>
+    <col min="1" max="1" width="24.42578125" style="1"/>
+    <col min="2" max="2" width="80.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="24.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -528,15 +558,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>5</v>
@@ -545,15 +575,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>5</v>
@@ -562,20 +592,37 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -587,18 +634,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{094BECEF-4844-4418-B6F1-0C40CA92EC6D}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="27.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="27.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="48.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -627,12 +674,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -641,7 +688,7 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>12</v>
@@ -656,18 +703,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
@@ -685,15 +732,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
@@ -702,73 +749,218 @@
         <v>11</v>
       </c>
       <c r="F4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="H4" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="E5" t="s">
         <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>24</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="E6" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>12</v>
+      <c r="F6" t="s">
+        <v>23</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="I6" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" s="3" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>